<commit_message>
Move B-cell GEO metadata
</commit_message>
<xml_diff>
--- a/GEO/Bcell_RNAseq_metadata.xlsx
+++ b/GEO/Bcell_RNAseq_metadata.xlsx
@@ -2844,19 +2844,19 @@
     <t xml:space="preserve">866f06eb64180eac67a72cff5d290ec7</t>
   </si>
   <si>
-    <t xml:space="preserve">female_Bcells.DEGs.csv</t>
+    <t xml:space="preserve">female_Bcells.DEGs.csv.gz</t>
   </si>
   <si>
     <t xml:space="preserve">CSV</t>
   </si>
   <si>
-    <t xml:space="preserve">ca47b9e118d40af4c4af97c2b7adf75d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">male_Bcells.DEGs.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7485f5ed88b26277b5d1f6fac1a55dd0</t>
+    <t xml:space="preserve">219d7a839ac13def5a36300e225e1693</t>
+  </si>
+  <si>
+    <t xml:space="preserve">male_Bcells.DEGs.csv.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">027c5b1ac1215ce04a44ff42f36a35a0</t>
   </si>
   <si>
     <t xml:space="preserve"># For each file listed in the "raw file" columns of the SAMPLES section above, provide additional information below.</t>
@@ -3650,7 +3650,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="35">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3683,14 +3683,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3715,10 +3707,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3740,10 +3728,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3759,20 +3743,12 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -3799,19 +3775,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3831,7 +3799,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 2" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -3904,24 +3872,24 @@
   </sheetPr>
   <dimension ref="A1:AV123"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B76" activeCellId="0" sqref="B76"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A81" activeCellId="0" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="36.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="1" width="28.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="1" width="28.65"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" s="5" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -3930,7 +3898,7 @@
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" s="5" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -3939,7 +3907,7 @@
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
-    <row r="4" s="5" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -3948,7 +3916,7 @@
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" s="5" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -3957,14 +3925,14 @@
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" s="5" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" s="8" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
@@ -3973,7 +3941,7 @@
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
     </row>
-    <row r="8" s="9" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -3982,974 +3950,964 @@
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" s="8" customFormat="true" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="s">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-    </row>
-    <row r="10" s="8" customFormat="true" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="s">
+      <c r="C9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+    </row>
+    <row r="10" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-    </row>
-    <row r="11" s="8" customFormat="true" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="s">
+      <c r="C10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+    </row>
+    <row r="11" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-    </row>
-    <row r="12" s="8" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="s">
+      <c r="C11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="12"/>
+      <c r="C12" s="10"/>
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
     </row>
-    <row r="13" s="8" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="15" t="s">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="12"/>
+      <c r="C13" s="10"/>
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
     </row>
-    <row r="14" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="15" t="s">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="12"/>
+      <c r="C14" s="10"/>
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
     </row>
-    <row r="15" s="8" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="15" t="s">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="10"/>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
     </row>
-    <row r="16" s="8" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="15" t="s">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="10"/>
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
     </row>
-    <row r="17" s="8" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="15"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="12"/>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="13"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="10"/>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
     </row>
-    <row r="18" s="8" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="7"/>
-      <c r="C18" s="12"/>
+      <c r="C18" s="10"/>
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
     </row>
-    <row r="19" s="9" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="17" t="s">
+    <row r="19" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" s="9" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="18" t="s">
+    <row r="20" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" s="9" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="19" t="s">
+    <row r="21" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
-    </row>
-    <row r="22" s="20" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="20" t="s">
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+    </row>
+    <row r="22" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="21" t="s">
+      <c r="D22" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="20" t="s">
+      <c r="E22" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="F22" s="20" t="s">
+      <c r="F22" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="G22" s="20" t="s">
+      <c r="G22" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="H22" s="20" t="s">
+      <c r="H22" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="I22" s="20" t="s">
+      <c r="I22" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="J22" s="20" t="s">
+      <c r="J22" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="K22" s="20" t="s">
+      <c r="K22" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="L22" s="20" t="s">
+      <c r="L22" s="17" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23" s="22" customFormat="true" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="22" t="s">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="22" t="s">
+      <c r="C23" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D23" s="22" t="s">
+      <c r="D23" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E23" s="23" t="s">
+      <c r="E23" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="F23" s="23" t="s">
+      <c r="F23" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="G23" s="23" t="s">
+      <c r="G23" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="H23" s="23" t="s">
+      <c r="H23" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="J23" s="23" t="s">
+      <c r="J23" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="K23" s="23" t="s">
+      <c r="K23" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="L23" s="23"/>
-    </row>
-    <row r="24" s="22" customFormat="true" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="22" t="s">
+      <c r="L23" s="19"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="22" t="s">
+      <c r="C24" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="22" t="s">
+      <c r="D24" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E24" s="23" t="s">
+      <c r="E24" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="F24" s="23" t="s">
+      <c r="F24" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="G24" s="23" t="s">
+      <c r="G24" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="H24" s="23" t="s">
+      <c r="H24" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="J24" s="23" t="s">
+      <c r="J24" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="K24" s="23" t="s">
+      <c r="K24" s="19" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" s="22" customFormat="true" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="22" t="s">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="C25" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="22" t="s">
+      <c r="D25" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E25" s="23" t="s">
+      <c r="E25" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="F25" s="23" t="s">
+      <c r="F25" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="G25" s="23" t="s">
+      <c r="G25" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="H25" s="23" t="s">
+      <c r="H25" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="J25" s="23" t="s">
+      <c r="J25" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="K25" s="23" t="s">
+      <c r="K25" s="19" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="22" t="s">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B26" s="22" t="s">
+      <c r="B26" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="22" t="s">
+      <c r="C26" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="22" t="s">
+      <c r="D26" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E26" s="23" t="s">
+      <c r="E26" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="F26" s="23" t="s">
+      <c r="F26" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="G26" s="23" t="s">
+      <c r="G26" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="H26" s="23" t="s">
+      <c r="H26" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="J26" s="23" t="s">
+      <c r="J26" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="K26" s="23" t="s">
+      <c r="K26" s="19" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="22" t="s">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="22" t="s">
+      <c r="C27" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D27" s="22" t="s">
+      <c r="D27" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E27" s="23" t="s">
+      <c r="E27" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="F27" s="23" t="s">
+      <c r="F27" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="G27" s="23" t="s">
+      <c r="G27" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="H27" s="23" t="s">
+      <c r="H27" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="J27" s="23" t="s">
+      <c r="J27" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="K27" s="23" t="s">
+      <c r="K27" s="19" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="22" t="s">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="22" t="s">
+      <c r="C28" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D28" s="22" t="s">
+      <c r="D28" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E28" s="23" t="s">
+      <c r="E28" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="F28" s="23" t="s">
+      <c r="F28" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="G28" s="23" t="s">
+      <c r="G28" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="H28" s="23" t="s">
+      <c r="H28" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="J28" s="23" t="s">
+      <c r="J28" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="K28" s="23" t="s">
+      <c r="K28" s="19" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="22" t="s">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="22" t="s">
+      <c r="C29" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="22" t="s">
+      <c r="D29" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E29" s="23" t="s">
+      <c r="E29" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="F29" s="23" t="s">
+      <c r="F29" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="G29" s="23" t="s">
+      <c r="G29" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="H29" s="23" t="s">
+      <c r="H29" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="J29" s="23" t="s">
+      <c r="J29" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="K29" s="23" t="s">
+      <c r="K29" s="19" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="22" t="s">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="22" t="s">
+      <c r="C30" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D30" s="22" t="s">
+      <c r="D30" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E30" s="23" t="s">
+      <c r="E30" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="F30" s="23" t="s">
+      <c r="F30" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="G30" s="23" t="s">
+      <c r="G30" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="H30" s="23" t="s">
+      <c r="H30" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="J30" s="23" t="s">
+      <c r="J30" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="K30" s="23" t="s">
+      <c r="K30" s="19" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="22" t="s">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B31" s="22" t="s">
+      <c r="B31" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="22" t="s">
+      <c r="C31" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D31" s="22" t="s">
+      <c r="D31" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E31" s="23" t="s">
+      <c r="E31" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="F31" s="23" t="s">
+      <c r="F31" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="G31" s="23" t="s">
+      <c r="G31" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="H31" s="23" t="s">
+      <c r="H31" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="J31" s="23" t="s">
+      <c r="J31" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="K31" s="23" t="s">
+      <c r="K31" s="19" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="22" t="s">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B32" s="22" t="s">
+      <c r="B32" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C32" s="22" t="s">
+      <c r="C32" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="22" t="s">
+      <c r="D32" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E32" s="23" t="s">
+      <c r="E32" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="F32" s="23" t="s">
+      <c r="F32" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="G32" s="23" t="s">
+      <c r="G32" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="H32" s="23" t="s">
+      <c r="H32" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="J32" s="23" t="s">
+      <c r="J32" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="K32" s="23" t="s">
+      <c r="K32" s="19" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="22" t="s">
+    <row r="33" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B33" s="22" t="s">
+      <c r="B33" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C33" s="22" t="s">
+      <c r="C33" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D33" s="22" t="s">
+      <c r="D33" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E33" s="23" t="s">
+      <c r="E33" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="F33" s="23" t="s">
+      <c r="F33" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="G33" s="23" t="s">
+      <c r="G33" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="H33" s="23" t="s">
+      <c r="H33" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="J33" s="23" t="s">
+      <c r="J33" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="K33" s="23" t="s">
+      <c r="K33" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="L33" s="23" t="s">
+      <c r="L33" s="19" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="22" t="s">
+    <row r="34" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B34" s="22" t="s">
+      <c r="B34" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C34" s="22" t="s">
+      <c r="C34" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D34" s="22" t="s">
+      <c r="D34" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E34" s="23" t="s">
+      <c r="E34" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="F34" s="23" t="s">
+      <c r="F34" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="G34" s="23" t="s">
+      <c r="G34" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="H34" s="23" t="s">
+      <c r="H34" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="J34" s="23" t="s">
+      <c r="J34" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="K34" s="23" t="s">
+      <c r="K34" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="L34" s="23" t="s">
+      <c r="L34" s="19" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="22" t="s">
+    <row r="35" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B35" s="22" t="s">
+      <c r="B35" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C35" s="22" t="s">
+      <c r="C35" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D35" s="22" t="s">
+      <c r="D35" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E35" s="23" t="s">
+      <c r="E35" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="F35" s="23" t="s">
+      <c r="F35" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="G35" s="23" t="s">
+      <c r="G35" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="H35" s="23" t="s">
+      <c r="H35" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="J35" s="23" t="s">
+      <c r="J35" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="K35" s="23" t="s">
+      <c r="K35" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="L35" s="23" t="s">
+      <c r="L35" s="19" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="22" t="s">
+    <row r="36" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B36" s="22" t="s">
+      <c r="B36" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C36" s="22" t="s">
+      <c r="C36" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D36" s="22" t="s">
+      <c r="D36" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E36" s="23" t="s">
+      <c r="E36" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="F36" s="23" t="s">
+      <c r="F36" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="G36" s="23" t="s">
+      <c r="G36" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="H36" s="23" t="s">
+      <c r="H36" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="J36" s="23" t="s">
+      <c r="J36" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="K36" s="23" t="s">
+      <c r="K36" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="L36" s="23" t="s">
+      <c r="L36" s="19" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="22" t="s">
+    <row r="37" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B37" s="22" t="s">
+      <c r="B37" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C37" s="22" t="s">
+      <c r="C37" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D37" s="22" t="s">
+      <c r="D37" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E37" s="23" t="s">
+      <c r="E37" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="F37" s="23" t="s">
+      <c r="F37" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="G37" s="23" t="s">
+      <c r="G37" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="H37" s="23" t="s">
+      <c r="H37" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="J37" s="23" t="s">
+      <c r="J37" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="K37" s="23" t="s">
+      <c r="K37" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="L37" s="23" t="s">
+      <c r="L37" s="19" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="22" t="s">
+    <row r="38" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B38" s="22" t="s">
+      <c r="B38" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C38" s="22" t="s">
+      <c r="C38" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D38" s="22" t="s">
+      <c r="D38" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E38" s="23" t="s">
+      <c r="E38" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="F38" s="23" t="s">
+      <c r="F38" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="G38" s="23" t="s">
+      <c r="G38" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="H38" s="23" t="s">
+      <c r="H38" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="J38" s="23" t="s">
+      <c r="J38" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="K38" s="23" t="s">
+      <c r="K38" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="L38" s="23" t="s">
+      <c r="L38" s="19" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="22" t="s">
+    <row r="39" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B39" s="22" t="s">
+      <c r="B39" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C39" s="22" t="s">
+      <c r="C39" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D39" s="22" t="s">
+      <c r="D39" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E39" s="23" t="s">
+      <c r="E39" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="F39" s="23" t="s">
+      <c r="F39" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="G39" s="23" t="s">
+      <c r="G39" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="H39" s="23" t="s">
+      <c r="H39" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="J39" s="23" t="s">
+      <c r="J39" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="K39" s="23" t="s">
+      <c r="K39" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="L39" s="23" t="s">
+      <c r="L39" s="19" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="22" t="s">
+    <row r="40" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C40" s="22" t="s">
+      <c r="C40" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D40" s="22" t="s">
+      <c r="D40" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E40" s="23" t="s">
+      <c r="E40" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="F40" s="23" t="s">
+      <c r="F40" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="G40" s="23" t="s">
+      <c r="G40" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="H40" s="23" t="s">
+      <c r="H40" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="J40" s="23" t="s">
+      <c r="J40" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="K40" s="23" t="s">
+      <c r="K40" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="L40" s="23" t="s">
+      <c r="L40" s="19" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="22"/>
-    </row>
-    <row r="42" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="22"/>
-    </row>
-    <row r="43" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="22"/>
-    </row>
-    <row r="44" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="24"/>
-    </row>
-    <row r="45" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="24"/>
-    </row>
-    <row r="46" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="24"/>
-    </row>
-    <row r="47" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="25" t="s">
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="20"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="20"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="20"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="B47" s="22"/>
-    </row>
-    <row r="48" s="5" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="48" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="5" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="15" t="s">
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="B49" s="26"/>
-      <c r="C49" s="26"/>
-      <c r="J49" s="26"/>
-      <c r="K49" s="26"/>
-    </row>
-    <row r="50" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="15" t="s">
+      <c r="B49" s="22"/>
+      <c r="C49" s="22"/>
+      <c r="J49" s="22"/>
+      <c r="K49" s="22"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="B50" s="26"/>
-      <c r="C50" s="26"/>
-      <c r="J50" s="26"/>
-      <c r="K50" s="26"/>
-    </row>
-    <row r="51" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="10" t="s">
+      <c r="B50" s="22"/>
+      <c r="C50" s="22"/>
+      <c r="J50" s="22"/>
+      <c r="K50" s="22"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="B51" s="26" t="s">
+      <c r="B51" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="C51" s="26"/>
-      <c r="J51" s="26"/>
-      <c r="K51" s="26"/>
-    </row>
-    <row r="52" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="10" t="s">
+      <c r="C51" s="22"/>
+      <c r="J51" s="22"/>
+      <c r="K51" s="22"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B52" s="26" t="s">
+      <c r="B52" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="C52" s="26"/>
-      <c r="J52" s="26"/>
-      <c r="K52" s="26"/>
-    </row>
-    <row r="53" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="10" t="s">
+      <c r="C52" s="22"/>
+      <c r="J52" s="22"/>
+      <c r="K52" s="22"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="B53" s="26" t="s">
+      <c r="B53" s="22" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="10"/>
-    </row>
-    <row r="55" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="8"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="6" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="56" s="27" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="27" t="s">
+    <row r="56" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="14" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="57" s="27" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="27" t="s">
+    <row r="57" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="14" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="10" t="s">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="B58" s="13" t="s">
+      <c r="B58" s="11" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="10" t="s">
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="B59" s="13" t="s">
+      <c r="B59" s="11" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="10" t="s">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="B60" s="13" t="s">
+      <c r="B60" s="11" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="10" t="s">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="B61" s="13" t="s">
+      <c r="B61" s="11" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="10" t="s">
+      <c r="A62" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="B62" s="28" t="s">
+      <c r="B62" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="C62" s="26"/>
-      <c r="J62" s="26"/>
-      <c r="K62" s="26"/>
+      <c r="C62" s="22"/>
+      <c r="J62" s="22"/>
+      <c r="K62" s="22"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="10" t="s">
+      <c r="A63" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="B63" s="29" t="s">
+      <c r="B63" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="C63" s="26"/>
-      <c r="J63" s="26"/>
-      <c r="K63" s="26"/>
+      <c r="C63" s="22"/>
+      <c r="J63" s="22"/>
+      <c r="K63" s="22"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="10" t="s">
+      <c r="A64" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="B64" s="30" t="s">
+      <c r="B64" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="C64" s="26"/>
-      <c r="J64" s="26"/>
-      <c r="K64" s="26"/>
+      <c r="C64" s="22"/>
+      <c r="J64" s="22"/>
+      <c r="K64" s="22"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="10" t="s">
+      <c r="A65" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B65" s="31" t="s">
+      <c r="B65" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="C65" s="26"/>
-      <c r="J65" s="26"/>
-      <c r="K65" s="26"/>
+      <c r="C65" s="22"/>
+      <c r="J65" s="22"/>
+      <c r="K65" s="22"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="10" t="s">
+      <c r="A66" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B66" s="31" t="s">
+      <c r="B66" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="C66" s="26"/>
-      <c r="J66" s="26"/>
-      <c r="K66" s="26"/>
+      <c r="C66" s="22"/>
+      <c r="J66" s="22"/>
+      <c r="K66" s="22"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="10" t="s">
+      <c r="A67" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B67" s="29" t="s">
+      <c r="B67" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="C67" s="26"/>
-      <c r="J67" s="26"/>
-      <c r="K67" s="26"/>
+      <c r="C67" s="22"/>
+      <c r="J67" s="22"/>
+      <c r="K67" s="22"/>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="10" t="s">
+      <c r="A68" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B68" s="29" t="s">
+      <c r="B68" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="C68" s="26"/>
-      <c r="J68" s="26"/>
-      <c r="K68" s="26"/>
-    </row>
-    <row r="69" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="10"/>
+      <c r="C68" s="22"/>
+      <c r="J68" s="22"/>
+      <c r="K68" s="22"/>
+    </row>
+    <row r="69" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="8"/>
       <c r="B69" s="0"/>
       <c r="C69" s="0"/>
       <c r="D69" s="0"/>
@@ -4998,741 +4956,719 @@
       <c r="AU69" s="0"/>
       <c r="AV69" s="0"/>
     </row>
-    <row r="70" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="27" t="s">
+    <row r="70" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="B70" s="27"/>
-      <c r="C70" s="27"/>
-      <c r="D70" s="27"/>
-      <c r="E70" s="27"/>
-      <c r="F70" s="27"/>
-      <c r="G70" s="27"/>
-      <c r="H70" s="27"/>
-      <c r="I70" s="27"/>
-      <c r="J70" s="27"/>
-      <c r="K70" s="27"/>
-      <c r="L70" s="27"/>
-      <c r="M70" s="27"/>
-      <c r="N70" s="27"/>
-      <c r="O70" s="27"/>
-      <c r="P70" s="27"/>
-      <c r="Q70" s="27"/>
-      <c r="R70" s="27"/>
-      <c r="S70" s="27"/>
-      <c r="T70" s="27"/>
-      <c r="U70" s="27"/>
-      <c r="V70" s="27"/>
-      <c r="W70" s="27"/>
-      <c r="X70" s="27"/>
-      <c r="Y70" s="27"/>
-      <c r="Z70" s="27"/>
-      <c r="AA70" s="27"/>
-      <c r="AB70" s="27"/>
-      <c r="AC70" s="27"/>
-      <c r="AD70" s="27"/>
-      <c r="AE70" s="27"/>
-      <c r="AF70" s="27"/>
-      <c r="AG70" s="27"/>
-      <c r="AH70" s="27"/>
-      <c r="AI70" s="27"/>
-      <c r="AJ70" s="27"/>
-      <c r="AK70" s="27"/>
-      <c r="AL70" s="27"/>
-      <c r="AM70" s="27"/>
-      <c r="AN70" s="27"/>
-      <c r="AO70" s="27"/>
-      <c r="AP70" s="27"/>
-      <c r="AQ70" s="27"/>
-      <c r="AR70" s="27"/>
-      <c r="AS70" s="27"/>
-      <c r="AT70" s="27"/>
-      <c r="AU70" s="27"/>
-      <c r="AV70" s="27"/>
-    </row>
-    <row r="71" s="33" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="32" t="s">
+      <c r="B70" s="14"/>
+      <c r="C70" s="14"/>
+      <c r="D70" s="14"/>
+      <c r="E70" s="14"/>
+      <c r="F70" s="14"/>
+      <c r="G70" s="14"/>
+      <c r="H70" s="14"/>
+      <c r="I70" s="14"/>
+      <c r="J70" s="14"/>
+      <c r="K70" s="14"/>
+      <c r="L70" s="14"/>
+      <c r="M70" s="14"/>
+      <c r="N70" s="14"/>
+      <c r="O70" s="14"/>
+      <c r="P70" s="14"/>
+      <c r="Q70" s="14"/>
+      <c r="R70" s="14"/>
+      <c r="S70" s="14"/>
+      <c r="T70" s="14"/>
+      <c r="U70" s="14"/>
+      <c r="V70" s="14"/>
+      <c r="W70" s="14"/>
+      <c r="X70" s="14"/>
+      <c r="Y70" s="14"/>
+      <c r="Z70" s="14"/>
+      <c r="AA70" s="14"/>
+      <c r="AB70" s="14"/>
+      <c r="AC70" s="14"/>
+      <c r="AD70" s="14"/>
+      <c r="AE70" s="14"/>
+      <c r="AF70" s="14"/>
+      <c r="AG70" s="14"/>
+      <c r="AH70" s="14"/>
+      <c r="AI70" s="14"/>
+      <c r="AJ70" s="14"/>
+      <c r="AK70" s="14"/>
+      <c r="AL70" s="14"/>
+      <c r="AM70" s="14"/>
+      <c r="AN70" s="14"/>
+      <c r="AO70" s="14"/>
+      <c r="AP70" s="14"/>
+      <c r="AQ70" s="14"/>
+      <c r="AR70" s="14"/>
+      <c r="AS70" s="14"/>
+      <c r="AT70" s="14"/>
+      <c r="AU70" s="14"/>
+      <c r="AV70" s="14"/>
+    </row>
+    <row r="71" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="B71" s="14"/>
-      <c r="C71" s="14"/>
-      <c r="D71" s="14"/>
-      <c r="E71" s="14"/>
-      <c r="F71" s="14"/>
-      <c r="G71" s="14"/>
-      <c r="H71" s="14"/>
-      <c r="I71" s="14"/>
-      <c r="J71" s="14"/>
-      <c r="K71" s="14"/>
-      <c r="L71" s="14"/>
-      <c r="M71" s="14"/>
-      <c r="N71" s="14"/>
-      <c r="O71" s="14"/>
-      <c r="P71" s="14"/>
-      <c r="Q71" s="14"/>
-      <c r="R71" s="14"/>
-      <c r="S71" s="14"/>
-      <c r="T71" s="14"/>
-      <c r="U71" s="14"/>
-      <c r="V71" s="14"/>
-      <c r="W71" s="14"/>
-      <c r="X71" s="14"/>
-      <c r="Y71" s="14"/>
-      <c r="Z71" s="14"/>
-      <c r="AA71" s="14"/>
-      <c r="AB71" s="14"/>
-      <c r="AC71" s="14"/>
-      <c r="AD71" s="14"/>
-      <c r="AE71" s="14"/>
-      <c r="AF71" s="14"/>
-      <c r="AG71" s="14"/>
-      <c r="AH71" s="14"/>
-      <c r="AI71" s="14"/>
-      <c r="AJ71" s="14"/>
-      <c r="AK71" s="14"/>
-      <c r="AL71" s="14"/>
-      <c r="AM71" s="14"/>
-      <c r="AN71" s="14"/>
-      <c r="AO71" s="14"/>
-      <c r="AP71" s="14"/>
-      <c r="AQ71" s="14"/>
-      <c r="AR71" s="14"/>
-      <c r="AS71" s="14"/>
-      <c r="AT71" s="14"/>
-      <c r="AU71" s="14"/>
-      <c r="AV71" s="14"/>
-    </row>
-    <row r="72" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="33" t="s">
+      <c r="B71" s="12"/>
+      <c r="C71" s="12"/>
+      <c r="D71" s="12"/>
+      <c r="E71" s="12"/>
+      <c r="F71" s="12"/>
+      <c r="G71" s="12"/>
+      <c r="H71" s="12"/>
+      <c r="I71" s="12"/>
+      <c r="J71" s="12"/>
+      <c r="K71" s="12"/>
+      <c r="L71" s="12"/>
+      <c r="M71" s="12"/>
+      <c r="N71" s="12"/>
+      <c r="O71" s="12"/>
+      <c r="P71" s="12"/>
+      <c r="Q71" s="12"/>
+      <c r="R71" s="12"/>
+      <c r="S71" s="12"/>
+      <c r="T71" s="12"/>
+      <c r="U71" s="12"/>
+      <c r="V71" s="12"/>
+      <c r="W71" s="12"/>
+      <c r="X71" s="12"/>
+      <c r="Y71" s="12"/>
+      <c r="Z71" s="12"/>
+      <c r="AA71" s="12"/>
+      <c r="AB71" s="12"/>
+      <c r="AC71" s="12"/>
+      <c r="AD71" s="12"/>
+      <c r="AE71" s="12"/>
+      <c r="AF71" s="12"/>
+      <c r="AG71" s="12"/>
+      <c r="AH71" s="12"/>
+      <c r="AI71" s="12"/>
+      <c r="AJ71" s="12"/>
+      <c r="AK71" s="12"/>
+      <c r="AL71" s="12"/>
+      <c r="AM71" s="12"/>
+      <c r="AN71" s="12"/>
+      <c r="AO71" s="12"/>
+      <c r="AP71" s="12"/>
+      <c r="AQ71" s="12"/>
+      <c r="AR71" s="12"/>
+      <c r="AS71" s="12"/>
+      <c r="AT71" s="12"/>
+      <c r="AU71" s="12"/>
+      <c r="AV71" s="12"/>
+    </row>
+    <row r="72" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="B72" s="33" t="s">
+      <c r="B72" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="C72" s="34" t="s">
+      <c r="C72" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="D72" s="33"/>
-      <c r="E72" s="33"/>
-      <c r="F72" s="33"/>
-      <c r="G72" s="33"/>
-      <c r="H72" s="33"/>
-      <c r="I72" s="33"/>
-      <c r="J72" s="33"/>
-      <c r="K72" s="33"/>
-      <c r="L72" s="33"/>
-      <c r="M72" s="33"/>
-      <c r="N72" s="33"/>
-      <c r="O72" s="33"/>
-      <c r="P72" s="33"/>
-      <c r="Q72" s="33"/>
-      <c r="R72" s="33"/>
-      <c r="S72" s="33"/>
-      <c r="T72" s="33"/>
-      <c r="U72" s="33"/>
-      <c r="V72" s="33"/>
-      <c r="W72" s="33"/>
-      <c r="X72" s="33"/>
-      <c r="Y72" s="33"/>
-      <c r="Z72" s="33"/>
-      <c r="AA72" s="33"/>
-      <c r="AB72" s="33"/>
-      <c r="AC72" s="33"/>
-      <c r="AD72" s="33"/>
-      <c r="AE72" s="33"/>
-      <c r="AF72" s="33"/>
-      <c r="AG72" s="33"/>
-      <c r="AH72" s="33"/>
-      <c r="AI72" s="33"/>
-      <c r="AJ72" s="33"/>
-      <c r="AK72" s="33"/>
-      <c r="AL72" s="33"/>
-      <c r="AM72" s="33"/>
-      <c r="AN72" s="33"/>
-      <c r="AO72" s="33"/>
-      <c r="AP72" s="33"/>
-      <c r="AQ72" s="33"/>
-      <c r="AR72" s="33"/>
-      <c r="AS72" s="33"/>
-      <c r="AT72" s="33"/>
-      <c r="AU72" s="33"/>
-      <c r="AV72" s="33"/>
-    </row>
-    <row r="73" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="22" t="s">
+      <c r="D72" s="27"/>
+      <c r="E72" s="27"/>
+      <c r="F72" s="27"/>
+      <c r="G72" s="27"/>
+      <c r="H72" s="27"/>
+      <c r="I72" s="27"/>
+      <c r="J72" s="27"/>
+      <c r="K72" s="27"/>
+      <c r="L72" s="27"/>
+      <c r="M72" s="27"/>
+      <c r="N72" s="27"/>
+      <c r="O72" s="27"/>
+      <c r="P72" s="27"/>
+      <c r="Q72" s="27"/>
+      <c r="R72" s="27"/>
+      <c r="S72" s="27"/>
+      <c r="T72" s="27"/>
+      <c r="U72" s="27"/>
+      <c r="V72" s="27"/>
+      <c r="W72" s="27"/>
+      <c r="X72" s="27"/>
+      <c r="Y72" s="27"/>
+      <c r="Z72" s="27"/>
+      <c r="AA72" s="27"/>
+      <c r="AB72" s="27"/>
+      <c r="AC72" s="27"/>
+      <c r="AD72" s="27"/>
+      <c r="AE72" s="27"/>
+      <c r="AF72" s="27"/>
+      <c r="AG72" s="27"/>
+      <c r="AH72" s="27"/>
+      <c r="AI72" s="27"/>
+      <c r="AJ72" s="27"/>
+      <c r="AK72" s="27"/>
+      <c r="AL72" s="27"/>
+      <c r="AM72" s="27"/>
+      <c r="AN72" s="27"/>
+      <c r="AO72" s="27"/>
+      <c r="AP72" s="27"/>
+      <c r="AQ72" s="27"/>
+      <c r="AR72" s="27"/>
+      <c r="AS72" s="27"/>
+      <c r="AT72" s="27"/>
+      <c r="AU72" s="27"/>
+      <c r="AV72" s="27"/>
+    </row>
+    <row r="73" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B73" s="14" t="s">
+      <c r="B73" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="C73" s="35" t="s">
+      <c r="C73" s="29" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="74" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="22" t="s">
+    <row r="74" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B74" s="14" t="s">
+      <c r="B74" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="C74" s="35" t="s">
+      <c r="C74" s="29" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="75" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="22" t="s">
+    <row r="75" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B75" s="16" t="s">
+      <c r="B75" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="C75" s="35" t="s">
+      <c r="C75" s="29" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="76" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="22" t="s">
+    <row r="76" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B76" s="16" t="s">
+      <c r="B76" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="C76" s="35" t="s">
+      <c r="C76" s="29" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="77" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="22"/>
-    </row>
-    <row r="78" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="22"/>
-    </row>
-    <row r="79" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="22"/>
-    </row>
-    <row r="80" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="22"/>
-    </row>
-    <row r="81" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="22"/>
+    <row r="77" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1"/>
+    </row>
+    <row r="78" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1"/>
+    </row>
+    <row r="79" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1"/>
+    </row>
+    <row r="80" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1"/>
+    </row>
+    <row r="81" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="1"/>
       <c r="B81" s="0"/>
       <c r="C81" s="0"/>
       <c r="D81" s="0"/>
       <c r="E81" s="0"/>
       <c r="F81" s="0"/>
     </row>
-    <row r="82" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="27" t="s">
+    <row r="82" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="B82" s="27"/>
-      <c r="C82" s="27"/>
-      <c r="D82" s="27"/>
-      <c r="E82" s="27"/>
-      <c r="F82" s="27"/>
-    </row>
-    <row r="83" s="34" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="32" t="s">
+      <c r="B82" s="14"/>
+      <c r="C82" s="14"/>
+      <c r="D82" s="14"/>
+      <c r="E82" s="14"/>
+      <c r="F82" s="14"/>
+    </row>
+    <row r="83" s="28" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="B83" s="14"/>
-      <c r="C83" s="14"/>
-      <c r="D83" s="32"/>
-      <c r="E83" s="14"/>
-      <c r="F83" s="14"/>
-    </row>
-    <row r="84" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="33" t="s">
+      <c r="B83" s="12"/>
+      <c r="C83" s="12"/>
+      <c r="D83" s="26"/>
+      <c r="E83" s="12"/>
+      <c r="F83" s="12"/>
+    </row>
+    <row r="84" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="B84" s="33" t="s">
+      <c r="B84" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="C84" s="34" t="s">
+      <c r="C84" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="D84" s="33" t="s">
+      <c r="D84" s="27" t="s">
         <v>146</v>
       </c>
-      <c r="E84" s="33" t="s">
+      <c r="E84" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="F84" s="33"/>
-    </row>
-    <row r="85" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="23" t="s">
+      <c r="F84" s="27"/>
+    </row>
+    <row r="85" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="B85" s="14" t="s">
+      <c r="B85" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="C85" s="35" t="s">
+      <c r="C85" s="29" t="s">
         <v>149</v>
       </c>
-      <c r="D85" s="14" t="s">
+      <c r="D85" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="E85" s="14" t="s">
+      <c r="E85" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="F85" s="16"/>
-    </row>
-    <row r="86" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="23" t="s">
+    </row>
+    <row r="86" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B86" s="14" t="s">
+      <c r="B86" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="C86" s="35" t="s">
+      <c r="C86" s="29" t="s">
         <v>152</v>
       </c>
-      <c r="D86" s="14" t="s">
+      <c r="D86" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="E86" s="14" t="s">
+      <c r="E86" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="F86" s="36"/>
-    </row>
-    <row r="87" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="23" t="s">
+      <c r="F86" s="30"/>
+    </row>
+    <row r="87" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="B87" s="14" t="s">
+      <c r="B87" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="C87" s="35" t="s">
+      <c r="C87" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="D87" s="14" t="s">
+      <c r="D87" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="E87" s="14" t="s">
+      <c r="E87" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="F87" s="16"/>
-    </row>
-    <row r="88" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="23" t="s">
+    </row>
+    <row r="88" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="B88" s="14" t="s">
+      <c r="B88" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="C88" s="35" t="s">
+      <c r="C88" s="29" t="s">
         <v>154</v>
       </c>
-      <c r="D88" s="14" t="s">
+      <c r="D88" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="E88" s="14" t="s">
+      <c r="E88" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="F88" s="36"/>
-    </row>
-    <row r="89" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="23" t="s">
+      <c r="F88" s="30"/>
+    </row>
+    <row r="89" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="B89" s="14" t="s">
+      <c r="B89" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="C89" s="35" t="s">
+      <c r="C89" s="29" t="s">
         <v>155</v>
       </c>
-      <c r="D89" s="14" t="s">
+      <c r="D89" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="E89" s="14" t="s">
+      <c r="E89" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="F89" s="36"/>
-    </row>
-    <row r="90" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="23" t="s">
+      <c r="F89" s="30"/>
+    </row>
+    <row r="90" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="B90" s="14" t="s">
+      <c r="B90" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="C90" s="35" t="s">
+      <c r="C90" s="29" t="s">
         <v>156</v>
       </c>
-      <c r="D90" s="14" t="s">
+      <c r="D90" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="E90" s="14" t="s">
+      <c r="E90" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="F90" s="16"/>
-    </row>
-    <row r="91" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="23" t="s">
+    </row>
+    <row r="91" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B91" s="14" t="s">
+      <c r="B91" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="C91" s="35" t="s">
+      <c r="C91" s="29" t="s">
         <v>157</v>
       </c>
-      <c r="D91" s="14" t="s">
+      <c r="D91" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="E91" s="14" t="s">
+      <c r="E91" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="F91" s="16"/>
-    </row>
-    <row r="92" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="23" t="s">
+    </row>
+    <row r="92" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="B92" s="14" t="s">
+      <c r="B92" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="C92" s="35" t="s">
+      <c r="C92" s="29" t="s">
         <v>158</v>
       </c>
-      <c r="D92" s="14" t="s">
+      <c r="D92" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="E92" s="14" t="s">
+      <c r="E92" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="F92" s="16"/>
-    </row>
-    <row r="93" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="23" t="s">
+    </row>
+    <row r="93" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="B93" s="14" t="s">
+      <c r="B93" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="C93" s="35" t="s">
+      <c r="C93" s="29" t="s">
         <v>159</v>
       </c>
-      <c r="D93" s="14" t="s">
+      <c r="D93" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="E93" s="14" t="s">
+      <c r="E93" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="F93" s="16"/>
-    </row>
-    <row r="94" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="23" t="s">
+    </row>
+    <row r="94" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="B94" s="14" t="s">
+      <c r="B94" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="C94" s="35" t="s">
+      <c r="C94" s="29" t="s">
         <v>160</v>
       </c>
-      <c r="D94" s="14" t="s">
+      <c r="D94" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="E94" s="14" t="s">
+      <c r="E94" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="F94" s="16"/>
-    </row>
-    <row r="95" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="23" t="s">
+    </row>
+    <row r="95" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="B95" s="14" t="s">
+      <c r="B95" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="C95" s="35" t="s">
+      <c r="C95" s="29" t="s">
         <v>161</v>
       </c>
-      <c r="D95" s="14" t="s">
+      <c r="D95" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="E95" s="16" t="s">
+      <c r="E95" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="F95" s="16"/>
-    </row>
-    <row r="96" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="23" t="s">
+    </row>
+    <row r="96" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="B96" s="14" t="s">
+      <c r="B96" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="C96" s="35" t="s">
+      <c r="C96" s="29" t="s">
         <v>163</v>
       </c>
-      <c r="D96" s="14" t="s">
+      <c r="D96" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="E96" s="16" t="s">
+      <c r="E96" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="F96" s="16"/>
-    </row>
-    <row r="97" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="23" t="s">
+    </row>
+    <row r="97" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="B97" s="14" t="s">
+      <c r="B97" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="C97" s="35" t="s">
+      <c r="C97" s="29" t="s">
         <v>164</v>
       </c>
-      <c r="D97" s="14" t="s">
+      <c r="D97" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="E97" s="16" t="s">
+      <c r="E97" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="F97" s="16"/>
-    </row>
-    <row r="98" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="23" t="s">
+    </row>
+    <row r="98" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="B98" s="14" t="s">
+      <c r="B98" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="C98" s="35" t="s">
+      <c r="C98" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="D98" s="14" t="s">
+      <c r="D98" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="E98" s="16" t="s">
+      <c r="E98" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="F98" s="16"/>
-    </row>
-    <row r="99" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="23" t="s">
+    </row>
+    <row r="99" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="B99" s="14" t="s">
+      <c r="B99" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="C99" s="35" t="s">
+      <c r="C99" s="29" t="s">
         <v>166</v>
       </c>
-      <c r="D99" s="14" t="s">
+      <c r="D99" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="E99" s="16" t="s">
+      <c r="E99" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="F99" s="16"/>
-    </row>
-    <row r="100" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="23" t="s">
+    </row>
+    <row r="100" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="B100" s="14" t="s">
+      <c r="B100" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="C100" s="35" t="s">
+      <c r="C100" s="29" t="s">
         <v>167</v>
       </c>
-      <c r="D100" s="14" t="s">
+      <c r="D100" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="E100" s="16" t="s">
+      <c r="E100" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="F100" s="16"/>
-    </row>
-    <row r="101" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="23" t="s">
+    </row>
+    <row r="101" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="B101" s="14" t="s">
+      <c r="B101" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="C101" s="35" t="s">
+      <c r="C101" s="29" t="s">
         <v>168</v>
       </c>
-      <c r="D101" s="14" t="s">
+      <c r="D101" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="E101" s="16" t="s">
+      <c r="E101" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="F101" s="36"/>
-    </row>
-    <row r="102" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="23" t="s">
+      <c r="F101" s="30"/>
+    </row>
+    <row r="102" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="B102" s="14" t="s">
+      <c r="B102" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="C102" s="35" t="s">
+      <c r="C102" s="29" t="s">
         <v>169</v>
       </c>
-      <c r="D102" s="14" t="s">
+      <c r="D102" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="E102" s="16" t="s">
+      <c r="E102" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="F102" s="16"/>
-    </row>
-    <row r="103" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="23" t="s">
+    </row>
+    <row r="103" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="B103" s="14" t="s">
+      <c r="B103" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="C103" s="35" t="s">
+      <c r="C103" s="29" t="s">
         <v>170</v>
       </c>
-      <c r="D103" s="14" t="s">
+      <c r="D103" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="E103" s="16" t="s">
+      <c r="E103" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="F103" s="36"/>
-    </row>
-    <row r="104" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="23" t="s">
+      <c r="F103" s="30"/>
+    </row>
+    <row r="104" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="B104" s="14" t="s">
+      <c r="B104" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="C104" s="35" t="s">
+      <c r="C104" s="29" t="s">
         <v>171</v>
       </c>
-      <c r="D104" s="14" t="s">
+      <c r="D104" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="E104" s="16" t="s">
+      <c r="E104" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="F104" s="16"/>
-    </row>
-    <row r="105" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="23" t="s">
+    </row>
+    <row r="105" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="B105" s="14" t="s">
+      <c r="B105" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="C105" s="35" t="s">
+      <c r="C105" s="29" t="s">
         <v>172</v>
       </c>
-      <c r="D105" s="14" t="s">
+      <c r="D105" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="E105" s="16" t="s">
+      <c r="E105" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="F105" s="16"/>
-    </row>
-    <row r="106" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="23" t="s">
+    </row>
+    <row r="106" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="B106" s="14" t="s">
+      <c r="B106" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="C106" s="35" t="s">
+      <c r="C106" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="D106" s="14" t="s">
+      <c r="D106" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="E106" s="16" t="s">
+      <c r="E106" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="F106" s="36"/>
-    </row>
-    <row r="107" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="23" t="s">
+      <c r="F106" s="30"/>
+    </row>
+    <row r="107" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="B107" s="14" t="s">
+      <c r="B107" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="C107" s="35" t="s">
+      <c r="C107" s="29" t="s">
         <v>174</v>
       </c>
-      <c r="D107" s="14" t="s">
+      <c r="D107" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="E107" s="16" t="s">
+      <c r="E107" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="F107" s="16"/>
-    </row>
-    <row r="108" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="23" t="s">
+    </row>
+    <row r="108" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="B108" s="14" t="s">
+      <c r="B108" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="C108" s="35" t="s">
+      <c r="C108" s="29" t="s">
         <v>175</v>
       </c>
-      <c r="D108" s="14" t="s">
+      <c r="D108" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="E108" s="16" t="s">
+      <c r="E108" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="F108" s="16"/>
-    </row>
-    <row r="109" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="23" t="s">
+    </row>
+    <row r="109" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="B109" s="14" t="s">
+      <c r="B109" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="C109" s="35" t="s">
+      <c r="C109" s="29" t="s">
         <v>176</v>
       </c>
-      <c r="D109" s="14" t="s">
+      <c r="D109" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="E109" s="16" t="s">
+      <c r="E109" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="F109" s="16"/>
-    </row>
-    <row r="110" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="23" t="s">
+    </row>
+    <row r="110" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="B110" s="14" t="s">
+      <c r="B110" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="C110" s="35" t="s">
+      <c r="C110" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="D110" s="14" t="s">
+      <c r="D110" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="E110" s="16" t="s">
+      <c r="E110" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="F110" s="16"/>
-    </row>
-    <row r="111" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F111" s="16"/>
-    </row>
-    <row r="112" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="14"/>
+    </row>
+    <row r="111" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="112" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="12"/>
       <c r="B112" s="0"/>
       <c r="C112" s="0"/>
       <c r="D112" s="0"/>
@@ -5740,107 +5676,107 @@
       <c r="F112" s="0"/>
       <c r="G112" s="0"/>
     </row>
-    <row r="113" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="27" t="s">
+    <row r="113" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="B113" s="27"/>
-      <c r="C113" s="27"/>
-      <c r="D113" s="27"/>
-      <c r="E113" s="27"/>
-      <c r="F113" s="27"/>
-      <c r="G113" s="27"/>
-    </row>
-    <row r="114" s="33" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="32" t="s">
+      <c r="B113" s="14"/>
+      <c r="C113" s="14"/>
+      <c r="D113" s="14"/>
+      <c r="E113" s="14"/>
+      <c r="F113" s="14"/>
+      <c r="G113" s="14"/>
+    </row>
+    <row r="114" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="26" t="s">
         <v>179</v>
       </c>
-      <c r="B114" s="14"/>
-      <c r="C114" s="14"/>
-      <c r="D114" s="14"/>
-      <c r="E114" s="14"/>
-      <c r="F114" s="14"/>
-      <c r="G114" s="14"/>
-    </row>
-    <row r="115" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="33" t="s">
+      <c r="B114" s="12"/>
+      <c r="C114" s="12"/>
+      <c r="D114" s="12"/>
+      <c r="E114" s="12"/>
+      <c r="F114" s="12"/>
+      <c r="G114" s="12"/>
+    </row>
+    <row r="115" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="27" t="s">
         <v>180</v>
       </c>
-      <c r="B115" s="33" t="s">
+      <c r="B115" s="27" t="s">
         <v>181</v>
       </c>
-      <c r="C115" s="33"/>
-      <c r="D115" s="33"/>
-      <c r="E115" s="33"/>
-      <c r="F115" s="33"/>
-      <c r="G115" s="33"/>
-    </row>
-    <row r="116" s="14" customFormat="true" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="23" t="s">
+      <c r="C115" s="27"/>
+      <c r="D115" s="27"/>
+      <c r="E115" s="27"/>
+      <c r="F115" s="27"/>
+      <c r="G115" s="27"/>
+    </row>
+    <row r="116" s="12" customFormat="true" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="B116" s="23" t="s">
+      <c r="B116" s="19" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="117" s="14" customFormat="true" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="23" t="s">
+    <row r="117" s="12" customFormat="true" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="B117" s="23" t="s">
+      <c r="B117" s="19" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="118" s="14" customFormat="true" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="23" t="s">
+    <row r="118" s="12" customFormat="true" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="B118" s="23" t="s">
+      <c r="B118" s="19" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="119" s="14" customFormat="true" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="23" t="s">
+    <row r="119" s="12" customFormat="true" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="B119" s="23" t="s">
+      <c r="B119" s="19" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="23" t="s">
+    <row r="120" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="B120" s="23" t="s">
+      <c r="B120" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="C120" s="14"/>
-      <c r="D120" s="14"/>
-      <c r="E120" s="14"/>
-      <c r="F120" s="14"/>
-      <c r="G120" s="14"/>
-    </row>
-    <row r="121" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="23" t="s">
+      <c r="C120" s="12"/>
+      <c r="D120" s="12"/>
+      <c r="E120" s="12"/>
+      <c r="F120" s="12"/>
+      <c r="G120" s="12"/>
+    </row>
+    <row r="121" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="B121" s="23" t="s">
+      <c r="B121" s="19" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="23" t="s">
+    <row r="122" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="B122" s="23" t="s">
+      <c r="B122" s="19" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="23" t="s">
+    <row r="123" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="B123" s="23" t="s">
+      <c r="B123" s="19" t="s">
         <v>103</v>
       </c>
     </row>
@@ -5875,7 +5811,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="40.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="1" width="28.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="1" width="28.65"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5931,7 +5867,7 @@
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" s="8" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
@@ -5941,7 +5877,7 @@
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
     </row>
-    <row r="8" s="9" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" s="5" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -5951,196 +5887,196 @@
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
     </row>
-    <row r="9" s="8" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="s">
+    <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-    </row>
-    <row r="10" s="8" customFormat="true" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="s">
+      <c r="C9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+    </row>
+    <row r="10" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="C10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-    </row>
-    <row r="11" s="8" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="s">
+      <c r="C10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+    </row>
+    <row r="11" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-    </row>
-    <row r="12" s="8" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="s">
+      <c r="C11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+    </row>
+    <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="C12" s="12"/>
+      <c r="C12" s="10"/>
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
     </row>
-    <row r="13" s="8" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10" t="s">
+    <row r="13" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="C13" s="12"/>
+      <c r="C13" s="10"/>
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
     </row>
-    <row r="14" s="8" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="15" t="s">
+    <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="10"/>
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
     </row>
-    <row r="15" s="8" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="15"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="12"/>
+    <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="13"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="10"/>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
       <c r="L15" s="7"/>
     </row>
-    <row r="16" s="8" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="7"/>
-      <c r="C16" s="12"/>
+      <c r="C16" s="10"/>
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
       <c r="L16" s="7"/>
     </row>
-    <row r="17" s="9" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="17" t="s">
+    <row r="17" s="5" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" s="9" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="18" t="s">
+    <row r="18" s="5" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" s="9" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="19" t="s">
+    <row r="19" s="5" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-    </row>
-    <row r="20" s="20" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="20" t="s">
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+    </row>
+    <row r="20" s="17" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="21" t="s">
+      <c r="D20" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E20" s="20" t="s">
+      <c r="E20" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="F20" s="20" t="s">
+      <c r="F20" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="G20" s="20" t="s">
+      <c r="G20" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="H20" s="20" t="s">
+      <c r="H20" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="I20" s="20" t="s">
+      <c r="I20" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="J20" s="20" t="s">
+      <c r="J20" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="K20" s="20" t="s">
+      <c r="K20" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="L20" s="20" t="s">
+      <c r="L20" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="M20" s="20" t="s">
+      <c r="M20" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="N20" s="20" t="s">
+      <c r="N20" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="O20" s="20" t="s">
+      <c r="O20" s="17" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" s="22" customFormat="true" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="22" t="s">
+    <row r="21" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="D21" s="22" t="s">
+      <c r="D21" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E21" s="22" t="s">
+      <c r="E21" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="F21" s="23" t="s">
+      <c r="F21" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="G21" s="22" t="s">
+      <c r="G21" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="H21" s="22" t="s">
+      <c r="H21" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="J21" s="22" t="s">
+      <c r="J21" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="L21" s="22" t="s">
+      <c r="L21" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="M21" s="22" t="s">
+      <c r="M21" s="1" t="s">
         <v>200</v>
       </c>
       <c r="N21" s="7" t="s">
@@ -6148,38 +6084,38 @@
       </c>
       <c r="O21" s="7"/>
     </row>
-    <row r="22" s="22" customFormat="true" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="22" t="s">
+    <row r="22" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C22" s="22" t="s">
+      <c r="C22" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="D22" s="22" t="s">
+      <c r="D22" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E22" s="22" t="s">
+      <c r="E22" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="F22" s="23" t="s">
+      <c r="F22" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="G22" s="22" t="s">
+      <c r="G22" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="H22" s="22" t="s">
+      <c r="H22" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="J22" s="22" t="s">
+      <c r="J22" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="L22" s="22" t="s">
+      <c r="L22" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="M22" s="22" t="s">
+      <c r="M22" s="1" t="s">
         <v>204</v>
       </c>
       <c r="N22" s="7" t="s">
@@ -6187,35 +6123,35 @@
       </c>
       <c r="O22" s="7"/>
     </row>
-    <row r="23" s="22" customFormat="true" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="22" t="s">
+    <row r="23" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="C23" s="22" t="s">
+      <c r="C23" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="D23" s="22" t="s">
+      <c r="D23" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E23" s="22" t="s">
+      <c r="E23" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="F23" s="23" t="s">
+      <c r="F23" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="G23" s="22" t="s">
+      <c r="G23" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="H23" s="22" t="s">
+      <c r="H23" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="J23" s="22" t="s">
+      <c r="J23" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="M23" s="22" t="s">
+      <c r="M23" s="1" t="s">
         <v>208</v>
       </c>
       <c r="N23" s="7" t="s">
@@ -6224,7 +6160,7 @@
       <c r="O23" s="7"/>
     </row>
     <row r="24" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -6262,13 +6198,12 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="24"/>
+      <c r="A25" s="20"/>
     </row>
     <row r="26" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="25" t="s">
+      <c r="A26" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="B26" s="22"/>
     </row>
     <row r="27" s="5" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
@@ -6276,55 +6211,55 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="B28" s="26" t="s">
+      <c r="B28" s="22" t="s">
         <v>215</v>
       </c>
-      <c r="C28" s="26"/>
-      <c r="J28" s="26"/>
-      <c r="K28" s="26"/>
-      <c r="L28" s="26"/>
+      <c r="C28" s="22"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
+      <c r="L28" s="22"/>
     </row>
     <row r="29" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="15" t="s">
+      <c r="A29" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="B29" s="26" t="s">
+      <c r="B29" s="22" t="s">
         <v>216</v>
       </c>
-      <c r="C29" s="26"/>
-      <c r="J29" s="26"/>
-      <c r="K29" s="26"/>
-      <c r="L29" s="26"/>
+      <c r="C29" s="22"/>
+      <c r="J29" s="22"/>
+      <c r="K29" s="22"/>
+      <c r="L29" s="22"/>
     </row>
     <row r="30" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="10" t="s">
+      <c r="A30" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="B30" s="26" t="s">
+      <c r="B30" s="22" t="s">
         <v>217</v>
       </c>
-      <c r="C30" s="26"/>
-      <c r="J30" s="26"/>
-      <c r="K30" s="26"/>
-      <c r="L30" s="26"/>
+      <c r="C30" s="22"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="22"/>
+      <c r="L30" s="22"/>
     </row>
     <row r="31" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B31" s="37" t="s">
+      <c r="B31" s="22" t="s">
         <v>218</v>
       </c>
-      <c r="C31" s="26"/>
-      <c r="J31" s="26"/>
-      <c r="K31" s="26"/>
-      <c r="L31" s="26"/>
+      <c r="C31" s="22"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="22"/>
+      <c r="L31" s="22"/>
     </row>
     <row r="32" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="10" t="s">
+      <c r="A32" s="8" t="s">
         <v>112</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -6332,25 +6267,25 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="10"/>
+      <c r="A33" s="8"/>
     </row>
     <row r="34" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="35" s="27" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="27" t="s">
+    <row r="35" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="14" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="36" s="27" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="27" t="s">
+    <row r="36" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="14" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="10" t="s">
+      <c r="A37" s="8" t="s">
         <v>117</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -6358,7 +6293,7 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="10" t="s">
+      <c r="A38" s="8" t="s">
         <v>117</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -6366,7 +6301,7 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="10" t="s">
+      <c r="A39" s="8" t="s">
         <v>117</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -6374,7 +6309,7 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="10" t="s">
+      <c r="A40" s="8" t="s">
         <v>117</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -6382,283 +6317,278 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="10" t="s">
+      <c r="A41" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="B41" s="30"/>
-      <c r="C41" s="26"/>
-      <c r="J41" s="26"/>
-      <c r="K41" s="26"/>
-      <c r="L41" s="26"/>
+      <c r="B41" s="22"/>
+      <c r="C41" s="22"/>
+      <c r="J41" s="22"/>
+      <c r="K41" s="22"/>
+      <c r="L41" s="22"/>
     </row>
     <row r="42" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="10" t="s">
+      <c r="A42" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="B42" s="30" t="s">
+      <c r="B42" s="22" t="s">
         <v>224</v>
       </c>
-      <c r="C42" s="26"/>
-      <c r="J42" s="26"/>
-      <c r="K42" s="26"/>
-      <c r="L42" s="26"/>
+      <c r="C42" s="22"/>
+      <c r="J42" s="22"/>
+      <c r="K42" s="22"/>
+      <c r="L42" s="22"/>
     </row>
     <row r="43" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B43" s="30" t="s">
+      <c r="B43" s="22" t="s">
         <v>225</v>
       </c>
-      <c r="C43" s="26"/>
-      <c r="J43" s="26"/>
-      <c r="K43" s="26"/>
-      <c r="L43" s="26"/>
+      <c r="C43" s="22"/>
+      <c r="J43" s="22"/>
+      <c r="K43" s="22"/>
+      <c r="L43" s="22"/>
     </row>
     <row r="44" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="10" t="s">
+      <c r="A44" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B44" s="30" t="s">
+      <c r="B44" s="22" t="s">
         <v>226</v>
       </c>
-      <c r="C44" s="26"/>
-      <c r="J44" s="26"/>
-      <c r="K44" s="26"/>
-      <c r="L44" s="26"/>
+      <c r="C44" s="22"/>
+      <c r="J44" s="22"/>
+      <c r="K44" s="22"/>
+      <c r="L44" s="22"/>
     </row>
     <row r="45" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="10"/>
-      <c r="B45" s="14"/>
-      <c r="C45" s="26"/>
-      <c r="J45" s="26"/>
-      <c r="K45" s="26"/>
-      <c r="L45" s="26"/>
-    </row>
-    <row r="46" s="27" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="27" t="s">
+      <c r="A45" s="8"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="22"/>
+      <c r="J45" s="22"/>
+      <c r="K45" s="22"/>
+      <c r="L45" s="22"/>
+    </row>
+    <row r="46" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="14" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="47" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="32" t="s">
+    <row r="47" s="12" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="26" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="48" s="33" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="33" t="s">
+    <row r="48" s="27" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="B48" s="33" t="s">
+      <c r="B48" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="C48" s="34" t="s">
+      <c r="C48" s="28" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="49" s="38" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="22" t="s">
+    <row r="49" s="31" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B49" s="16" t="s">
+      <c r="B49" s="12" t="s">
         <v>227</v>
       </c>
-      <c r="C49" s="22" t="s">
+      <c r="C49" s="1" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="50" s="38" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="22" t="s">
+    <row r="50" s="31" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B50" s="16" t="s">
+      <c r="B50" s="12" t="s">
         <v>227</v>
       </c>
-      <c r="C50" s="22" t="s">
+      <c r="C50" s="1" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="51" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="22" t="s">
+    <row r="51" s="12" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B51" s="14" t="s">
+      <c r="B51" s="12" t="s">
         <v>227</v>
       </c>
-      <c r="C51" s="22" t="s">
+      <c r="C51" s="1" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="52" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="22" t="s">
+    <row r="52" s="12" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B52" s="14" t="s">
+      <c r="B52" s="12" t="s">
         <v>231</v>
       </c>
-      <c r="C52" s="22" t="s">
+      <c r="C52" s="1" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="53" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="22" t="s">
+    <row r="53" s="12" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B53" s="14" t="s">
+      <c r="B53" s="12" t="s">
         <v>231</v>
       </c>
-      <c r="C53" s="22" t="s">
+      <c r="C53" s="1" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="54" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="22" t="s">
+    <row r="54" s="12" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B54" s="14" t="s">
+      <c r="B54" s="12" t="s">
         <v>231</v>
       </c>
-      <c r="C54" s="22" t="s">
+      <c r="C54" s="1" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="55" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="22" t="s">
+    <row r="55" s="12" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="B55" s="14" t="s">
+      <c r="B55" s="12" t="s">
         <v>231</v>
       </c>
-      <c r="C55" s="22" t="s">
+      <c r="C55" s="1" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="56" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="22"/>
-      <c r="C56" s="22"/>
-    </row>
-    <row r="57" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="22"/>
-    </row>
-    <row r="58" s="27" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="27" t="s">
+    <row r="56" s="12" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+    </row>
+    <row r="57" s="12" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1"/>
+    </row>
+    <row r="58" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="14" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="59" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="32" t="s">
+    <row r="59" s="12" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="D59" s="32"/>
-    </row>
-    <row r="60" s="34" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="33" t="s">
+      <c r="D59" s="26"/>
+    </row>
+    <row r="60" s="28" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="B60" s="33" t="s">
+      <c r="B60" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="C60" s="34" t="s">
+      <c r="C60" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="D60" s="33" t="s">
+      <c r="D60" s="27" t="s">
         <v>146</v>
       </c>
-      <c r="E60" s="33" t="s">
+      <c r="E60" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="F60" s="33"/>
-    </row>
-    <row r="61" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F60" s="27"/>
+    </row>
+    <row r="61" s="12" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="B61" s="22" t="s">
+      <c r="B61" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C61" s="22" t="s">
+      <c r="C61" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="D61" s="22" t="s">
+      <c r="D61" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="E61" s="16" t="s">
+      <c r="E61" s="12" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="62" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" s="12" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="B62" s="22" t="s">
+      <c r="B62" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C62" s="22" t="s">
+      <c r="C62" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="D62" s="22" t="s">
+      <c r="D62" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="E62" s="16" t="s">
+      <c r="E62" s="12" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="63" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" s="12" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="B63" s="22" t="s">
+      <c r="B63" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C63" s="22" t="s">
+      <c r="C63" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="D63" s="22" t="s">
+      <c r="D63" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="E63" s="16" t="s">
+      <c r="E63" s="12" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="64" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="14" t="s">
+    <row r="64" s="12" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="B64" s="22" t="s">
+      <c r="B64" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C64" s="22" t="s">
+      <c r="C64" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="D64" s="22" t="s">
+      <c r="D64" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="E64" s="16" t="s">
+      <c r="E64" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="F64" s="16"/>
-    </row>
-    <row r="65" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F65" s="16"/>
-    </row>
-    <row r="66" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F66" s="16"/>
-    </row>
-    <row r="67" s="27" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="27" t="s">
+    </row>
+    <row r="65" s="12" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="66" s="12" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="67" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="14" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="68" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="32" t="s">
+    <row r="68" s="12" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="26" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="69" s="33" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="33" t="s">
+    <row r="69" s="27" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="27" t="s">
         <v>180</v>
       </c>
-      <c r="B69" s="33" t="s">
+      <c r="B69" s="27" t="s">
         <v>181</v>
       </c>
     </row>
@@ -6744,7 +6674,7 @@
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" s="8" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
@@ -6753,7 +6683,7 @@
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
     </row>
-    <row r="8" s="9" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" s="5" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -6762,220 +6692,220 @@
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" s="8" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="s">
+    <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-    </row>
-    <row r="10" s="8" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="s">
+      <c r="C9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+    </row>
+    <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="C10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-    </row>
-    <row r="11" s="8" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="s">
+      <c r="C10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+    </row>
+    <row r="11" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-    </row>
-    <row r="12" s="8" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="s">
+      <c r="C11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+    </row>
+    <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-    </row>
-    <row r="13" s="8" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10" t="s">
+      <c r="C12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+    </row>
+    <row r="13" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-    </row>
-    <row r="14" s="8" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10" t="s">
+      <c r="C13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+    </row>
+    <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="C14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-    </row>
-    <row r="15" s="8" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="10" t="s">
+      <c r="C14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+    </row>
+    <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="12" t="s">
         <v>246</v>
       </c>
-      <c r="C15" s="12"/>
+      <c r="C15" s="10"/>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
     </row>
-    <row r="16" s="8" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10" t="s">
+    <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="12" t="s">
         <v>247</v>
       </c>
-      <c r="C16" s="12"/>
+      <c r="C16" s="10"/>
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
     </row>
-    <row r="17" s="8" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="15" t="s">
+    <row r="17" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="12" t="s">
         <v>248</v>
       </c>
-      <c r="C17" s="12"/>
+      <c r="C17" s="10"/>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
     </row>
-    <row r="18" s="8" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="15"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="12"/>
+    <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="13"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="10"/>
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
     </row>
-    <row r="19" s="8" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="7"/>
-      <c r="C19" s="12"/>
+      <c r="C19" s="10"/>
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
     </row>
-    <row r="20" s="9" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="17" t="s">
+    <row r="20" s="5" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" s="9" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="18" t="s">
+    <row r="21" s="5" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" s="9" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="19" t="s">
+    <row r="22" s="5" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-    </row>
-    <row r="23" s="20" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="20" t="s">
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+    </row>
+    <row r="23" s="17" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="21" t="s">
+      <c r="D23" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E23" s="20" t="s">
+      <c r="E23" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="F23" s="20" t="s">
+      <c r="F23" s="17" t="s">
         <v>249</v>
       </c>
-      <c r="G23" s="20" t="s">
+      <c r="G23" s="17" t="s">
         <v>250</v>
       </c>
-      <c r="H23" s="20" t="s">
+      <c r="H23" s="17" t="s">
         <v>251</v>
       </c>
-      <c r="I23" s="20" t="s">
+      <c r="I23" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="J23" s="20" t="s">
+      <c r="J23" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="K23" s="20" t="s">
+      <c r="K23" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="L23" s="20" t="s">
+      <c r="L23" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="M23" s="20" t="s">
+      <c r="M23" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="N23" s="20" t="s">
+      <c r="N23" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="O23" s="20" t="s">
+      <c r="O23" s="17" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" s="22" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="22" t="s">
+    <row r="24" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="C24" s="39" t="s">
+      <c r="C24" s="32" t="s">
         <v>253</v>
       </c>
-      <c r="D24" s="22" t="s">
+      <c r="D24" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E24" s="22" t="s">
+      <c r="E24" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F24" s="22" t="s">
+      <c r="F24" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="G24" s="22" t="s">
+      <c r="G24" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="H24" s="22" t="s">
+      <c r="H24" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="K24" s="22" t="s">
+      <c r="K24" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="M24" s="22" t="s">
+      <c r="M24" s="1" t="s">
         <v>258</v>
       </c>
       <c r="N24" s="7" t="s">
@@ -6988,100 +6918,100 @@
       <c r="Q24" s="7"/>
       <c r="R24" s="7"/>
     </row>
-    <row r="25" s="22" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="22" t="s">
+    <row r="25" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="C25" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="D25" s="22" t="s">
+      <c r="D25" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E25" s="22" t="s">
+      <c r="E25" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F25" s="22" t="s">
+      <c r="F25" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="G25" s="22" t="s">
+      <c r="G25" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="H25" s="22" t="s">
+      <c r="H25" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="K25" s="22" t="s">
+      <c r="K25" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="M25" s="22" t="s">
+      <c r="M25" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="N25" s="40" t="s">
+      <c r="N25" s="33" t="s">
         <v>262</v>
       </c>
-      <c r="O25" s="40" t="s">
+      <c r="O25" s="33" t="s">
         <v>262</v>
       </c>
-      <c r="P25" s="41"/>
-    </row>
-    <row r="26" s="22" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="22" t="s">
+      <c r="P25" s="33"/>
+    </row>
+    <row r="26" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="39" t="s">
+      <c r="B26" s="32" t="s">
         <v>263</v>
       </c>
-      <c r="C26" s="22" t="s">
+      <c r="C26" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="D26" s="22" t="s">
+      <c r="D26" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E26" s="22" t="s">
+      <c r="E26" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F26" s="22" t="s">
+      <c r="F26" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="G26" s="22" t="s">
+      <c r="G26" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="H26" s="22" t="s">
+      <c r="H26" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="K26" s="22" t="s">
+      <c r="K26" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="M26" s="22" t="s">
+      <c r="M26" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="N26" s="22" t="s">
+      <c r="N26" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="O26" s="22" t="s">
+      <c r="O26" s="1" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="39" t="s">
+      <c r="B27" s="32" t="s">
         <v>268</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="D27" s="22" t="s">
+      <c r="D27" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F27" s="22" t="s">
+      <c r="F27" s="1" t="s">
         <v>254</v>
       </c>
       <c r="G27" s="1" t="s">
@@ -7090,10 +7020,10 @@
       <c r="H27" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="K27" s="22" t="s">
+      <c r="K27" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="M27" s="22" t="s">
+      <c r="M27" s="1" t="s">
         <v>269</v>
       </c>
       <c r="N27" s="7" t="s">
@@ -7103,14 +7033,10 @@
         <v>271</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="22"/>
-    </row>
     <row r="29" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="B29" s="22"/>
     </row>
     <row r="30" s="5" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
@@ -7118,47 +7044,47 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="15" t="s">
+      <c r="A31" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="B31" s="14"/>
-      <c r="C31" s="26"/>
-      <c r="J31" s="26"/>
-      <c r="K31" s="26"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="22"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="22"/>
     </row>
     <row r="32" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="15" t="s">
+      <c r="A32" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="B32" s="26"/>
-      <c r="C32" s="26"/>
-      <c r="J32" s="26"/>
-      <c r="K32" s="26"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="22"/>
+      <c r="J32" s="22"/>
+      <c r="K32" s="22"/>
     </row>
     <row r="33" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="10" t="s">
+      <c r="A33" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="B33" s="26" t="s">
+      <c r="B33" s="22" t="s">
         <v>272</v>
       </c>
-      <c r="C33" s="26"/>
-      <c r="J33" s="26"/>
-      <c r="K33" s="26"/>
+      <c r="C33" s="22"/>
+      <c r="J33" s="22"/>
+      <c r="K33" s="22"/>
     </row>
     <row r="34" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="10" t="s">
+      <c r="A34" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="12" t="s">
         <v>273</v>
       </c>
-      <c r="C34" s="26"/>
-      <c r="J34" s="26"/>
-      <c r="K34" s="26"/>
+      <c r="C34" s="22"/>
+      <c r="J34" s="22"/>
+      <c r="K34" s="22"/>
     </row>
     <row r="35" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="8" t="s">
         <v>112</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -7166,25 +7092,25 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="10"/>
+      <c r="A36" s="8"/>
     </row>
     <row r="37" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="38" s="27" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="27" t="s">
+    <row r="38" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="14" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="39" s="27" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="27" t="s">
+    <row r="39" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="14" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="10" t="s">
+      <c r="A40" s="8" t="s">
         <v>117</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -7192,7 +7118,7 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="10" t="s">
+      <c r="A41" s="8" t="s">
         <v>117</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -7200,7 +7126,7 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="10" t="s">
+      <c r="A42" s="8" t="s">
         <v>117</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -7208,334 +7134,331 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="B43" s="22"/>
     </row>
     <row r="44" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="10" t="s">
+      <c r="A44" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="B44" s="30"/>
-      <c r="C44" s="26"/>
-      <c r="J44" s="26"/>
-      <c r="K44" s="26"/>
+      <c r="B44" s="22"/>
+      <c r="C44" s="22"/>
+      <c r="J44" s="22"/>
+      <c r="K44" s="22"/>
     </row>
     <row r="45" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="10" t="s">
+      <c r="A45" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="B45" s="30" t="s">
+      <c r="B45" s="22" t="s">
         <v>224</v>
       </c>
-      <c r="C45" s="26"/>
-      <c r="J45" s="26"/>
-      <c r="K45" s="26"/>
+      <c r="C45" s="22"/>
+      <c r="J45" s="22"/>
+      <c r="K45" s="22"/>
     </row>
     <row r="46" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="10" t="s">
+      <c r="A46" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B46" s="30" t="s">
+      <c r="B46" s="22" t="s">
         <v>278</v>
       </c>
-      <c r="C46" s="26"/>
-      <c r="J46" s="26"/>
-      <c r="K46" s="26"/>
+      <c r="C46" s="22"/>
+      <c r="J46" s="22"/>
+      <c r="K46" s="22"/>
     </row>
     <row r="47" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="10" t="s">
+      <c r="A47" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B47" s="30" t="s">
+      <c r="B47" s="22" t="s">
         <v>279</v>
       </c>
-      <c r="C47" s="26"/>
-      <c r="J47" s="26"/>
-      <c r="K47" s="26"/>
+      <c r="C47" s="22"/>
+      <c r="J47" s="22"/>
+      <c r="K47" s="22"/>
     </row>
     <row r="48" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="10"/>
-      <c r="B48" s="14"/>
-      <c r="C48" s="26"/>
-      <c r="J48" s="26"/>
-      <c r="K48" s="26"/>
-    </row>
-    <row r="49" s="27" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="27" t="s">
+      <c r="A48" s="8"/>
+      <c r="B48" s="12"/>
+      <c r="C48" s="22"/>
+      <c r="J48" s="22"/>
+      <c r="K48" s="22"/>
+    </row>
+    <row r="49" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="14" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="50" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="32" t="s">
+    <row r="50" s="12" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="26" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="51" s="33" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="33" t="s">
+    <row r="51" s="27" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="B51" s="33" t="s">
+      <c r="B51" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="C51" s="34" t="s">
+      <c r="C51" s="28" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="52" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="22" t="s">
+    <row r="52" s="12" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="B52" s="22" t="s">
+      <c r="B52" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="C52" s="22" t="s">
+      <c r="C52" s="1" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="53" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="22" t="s">
+    <row r="53" s="12" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="B53" s="22" t="s">
+      <c r="B53" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="C53" s="22" t="s">
+      <c r="C53" s="1" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="54" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="22" t="s">
+    <row r="54" s="12" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="B54" s="22" t="s">
+      <c r="B54" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="C54" s="22" t="s">
+      <c r="C54" s="1" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="55" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="22" t="s">
+    <row r="55" s="12" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="B55" s="22" t="s">
+      <c r="B55" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="C55" s="22" t="s">
+      <c r="C55" s="1" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="56" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="22" t="s">
+    <row r="56" s="12" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="B56" s="22" t="s">
+      <c r="B56" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="C56" s="22" t="s">
+      <c r="C56" s="1" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="57" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="22"/>
-      <c r="B57" s="22"/>
-      <c r="C57" s="22"/>
-    </row>
-    <row r="58" s="27" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="27" t="s">
+    <row r="57" s="12" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+    </row>
+    <row r="58" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="14" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="59" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="32" t="s">
+    <row r="59" s="12" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="D59" s="32"/>
-    </row>
-    <row r="60" s="34" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="33" t="s">
+      <c r="D59" s="26"/>
+    </row>
+    <row r="60" s="28" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="B60" s="33" t="s">
+      <c r="B60" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="C60" s="34" t="s">
+      <c r="C60" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="D60" s="33" t="s">
+      <c r="D60" s="27" t="s">
         <v>146</v>
       </c>
-      <c r="E60" s="33" t="s">
+      <c r="E60" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="F60" s="33"/>
-    </row>
-    <row r="61" s="42" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F60" s="27"/>
+    </row>
+    <row r="61" s="34" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="B61" s="22" t="s">
+      <c r="B61" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C61" s="22" t="s">
+      <c r="C61" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="D61" s="40" t="s">
+      <c r="D61" s="33" t="s">
         <v>286</v>
       </c>
-      <c r="E61" s="16" t="s">
+      <c r="E61" s="12" t="s">
         <v>287</v>
       </c>
-      <c r="F61" s="38"/>
-    </row>
-    <row r="62" s="42" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F61" s="31"/>
+    </row>
+    <row r="62" s="34" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="7" t="s">
         <v>288</v>
       </c>
-      <c r="B62" s="22" t="s">
+      <c r="B62" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C62" s="22" t="s">
+      <c r="C62" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="D62" s="40" t="s">
+      <c r="D62" s="33" t="s">
         <v>286</v>
       </c>
-      <c r="E62" s="16" t="s">
+      <c r="E62" s="12" t="s">
         <v>287</v>
       </c>
-      <c r="F62" s="38"/>
-    </row>
-    <row r="63" s="42" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F62" s="31"/>
+    </row>
+    <row r="63" s="34" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="7" t="s">
         <v>262</v>
       </c>
-      <c r="B63" s="22" t="s">
+      <c r="B63" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C63" s="22" t="s">
+      <c r="C63" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="D63" s="40" t="s">
+      <c r="D63" s="33" t="s">
         <v>286</v>
       </c>
-      <c r="E63" s="16" t="s">
+      <c r="E63" s="12" t="s">
         <v>287</v>
       </c>
-      <c r="F63" s="38"/>
-    </row>
-    <row r="64" s="42" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F63" s="31"/>
+    </row>
+    <row r="64" s="34" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="7" t="s">
         <v>289</v>
       </c>
-      <c r="B64" s="22" t="s">
+      <c r="B64" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C64" s="22" t="s">
+      <c r="C64" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="D64" s="40" t="s">
+      <c r="D64" s="33" t="s">
         <v>286</v>
       </c>
-      <c r="E64" s="16" t="s">
+      <c r="E64" s="12" t="s">
         <v>287</v>
       </c>
-      <c r="F64" s="38"/>
-    </row>
-    <row r="65" s="42" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F64" s="31"/>
+    </row>
+    <row r="65" s="34" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="7" t="s">
         <v>266</v>
       </c>
-      <c r="B65" s="22" t="s">
+      <c r="B65" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C65" s="22" t="s">
+      <c r="C65" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="D65" s="40" t="s">
+      <c r="D65" s="33" t="s">
         <v>286</v>
       </c>
-      <c r="E65" s="16" t="s">
+      <c r="E65" s="12" t="s">
         <v>287</v>
       </c>
-      <c r="F65" s="38"/>
-    </row>
-    <row r="66" s="42" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F65" s="31"/>
+    </row>
+    <row r="66" s="34" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="7" t="s">
         <v>267</v>
       </c>
-      <c r="B66" s="22" t="s">
+      <c r="B66" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C66" s="22" t="s">
+      <c r="C66" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="D66" s="40" t="s">
+      <c r="D66" s="33" t="s">
         <v>286</v>
       </c>
-      <c r="E66" s="16" t="s">
+      <c r="E66" s="12" t="s">
         <v>287</v>
       </c>
-      <c r="F66" s="38"/>
-    </row>
-    <row r="67" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F66" s="31"/>
+    </row>
+    <row r="67" s="12" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="7" t="s">
         <v>270</v>
       </c>
-      <c r="B67" s="22" t="s">
+      <c r="B67" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C67" s="22" t="s">
+      <c r="C67" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="D67" s="40" t="s">
+      <c r="D67" s="33" t="s">
         <v>286</v>
       </c>
-      <c r="E67" s="16" t="s">
+      <c r="E67" s="12" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="68" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" s="12" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="7" t="s">
         <v>271</v>
       </c>
-      <c r="B68" s="22" t="s">
+      <c r="B68" s="1" t="s">
         <v>148</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="D68" s="40" t="s">
+      <c r="D68" s="33" t="s">
         <v>286</v>
       </c>
-      <c r="E68" s="16" t="s">
+      <c r="E68" s="12" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="69" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F69" s="16"/>
-    </row>
-    <row r="70" s="27" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="27" t="s">
+    <row r="69" s="12" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="70" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="14" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="71" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="32" t="s">
+    <row r="71" s="12" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="26" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="72" s="33" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="33" t="s">
+    <row r="72" s="27" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="27" t="s">
         <v>180</v>
       </c>
-      <c r="B72" s="33" t="s">
+      <c r="B72" s="27" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="73" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" s="12" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="7" t="s">
         <v>259</v>
       </c>
@@ -7543,7 +7466,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="74" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" s="12" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="7" t="s">
         <v>262</v>
       </c>
@@ -7551,7 +7474,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="75" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" s="12" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="7" t="s">
         <v>266</v>
       </c>
@@ -7559,7 +7482,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="76" s="14" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" s="12" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="7" t="s">
         <v>270</v>
       </c>

</xml_diff>